<commit_message>
PSD comments zichtbaar gemaakt
</commit_message>
<xml_diff>
--- a/opdracht_1.3 commentaar/PSD commentaar.xlsx
+++ b/opdracht_1.3 commentaar/PSD commentaar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bitnami\wampstack-7.1.25-0\apache2\htdocs\Bart\opdracht_1.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bitnami\wampstack-7.1.30-0\apache2\htdocs\Educom_Curriculum\opdracht_1.3 commentaar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71AF533-CED2-4710-B2CD-90590269AD8F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD94FC40-81A8-4F3C-9FBD-9CAD58409110}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="21600" windowHeight="11220" xr2:uid="{04326905-C870-4FF9-AE2C-65228360DEC8}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{04326905-C870-4FF9-AE2C-65228360DEC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,34 +43,70 @@
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9655CEA5-C341-42BD-A14A-B51E0AF8AF10}">
       <text>
-        <t>[Opmerkingenthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
 Opmerking:
     Mis hier test voor request type == POST</t>
+        </r>
       </text>
     </comment>
     <comment ref="D29" authorId="1" shapeId="0" xr:uid="{B1B0F78C-E12F-4B12-8112-FF1EBCD6D8A6}">
       <text>
-        <t>[Opmerkingenthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
 Opmerking:
     Mis hiervoor een test of alle error messages leeg zijn (in dat geval wordt de bedankt pagina getoond)</t>
+        </r>
       </text>
     </comment>
     <comment ref="D47" authorId="2" shapeId="0" xr:uid="{2CC1F27A-DB95-461F-862B-0298A5C8E7EE}">
       <text>
-        <t>[Opmerkingenthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
 Opmerking:
     Deze test moet op regel 29</t>
+        </r>
       </text>
     </comment>
     <comment ref="C50" authorId="3" shapeId="0" xr:uid="{A8AA35B0-D09F-459B-BE68-1D9CF6D58432}">
       <text>
-        <t>[Opmerkingenthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
 Opmerking:
     De opdracht was niet below form, maar in plaats van form</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -126,19 +162,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -356,18 +386,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -386,14 +484,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="787C82"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="3F4246"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -701,24 +799,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBA19C7-7F96-4E1E-A2FD-2C34D1CD4EFC}">
   <dimension ref="C1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:21" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:21" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -734,13 +832,13 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="I3" s="1"/>
@@ -757,7 +855,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="b">
         <v>1</v>
       </c>
@@ -782,7 +880,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
@@ -801,7 +899,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C6" s="18"/>
       <c r="D6" s="19"/>
       <c r="E6" s="20"/>
@@ -816,7 +914,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C7" s="18"/>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
@@ -831,7 +929,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C8" s="18"/>
       <c r="D8" s="19"/>
       <c r="E8" s="20"/>
@@ -848,7 +946,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="20"/>
@@ -863,7 +961,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="21"/>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -878,14 +976,14 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -895,13 +993,13 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
       <c r="I12" s="1"/>
@@ -912,7 +1010,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="b">
         <v>1</v>
       </c>
@@ -931,7 +1029,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
         <v>8</v>
       </c>
@@ -950,7 +1048,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
@@ -965,7 +1063,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" s="18"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
@@ -980,7 +1078,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
@@ -997,7 +1095,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20"/>
@@ -1012,7 +1110,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
@@ -1026,27 +1124,27 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="24"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="6"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="b">
         <v>1</v>
       </c>
@@ -1058,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1168,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
       <c r="E24" s="20"/>
@@ -1078,7 +1176,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
       <c r="E25" s="20"/>
@@ -1086,7 +1184,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
       <c r="E26" s="20"/>
@@ -1096,7 +1194,7 @@
       <c r="G26" s="16"/>
       <c r="H26" s="17"/>
     </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C27" s="18"/>
       <c r="D27" s="19"/>
       <c r="E27" s="20"/>
@@ -1104,7 +1202,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C28" s="21"/>
       <c r="D28" s="22"/>
       <c r="E28" s="23"/>
@@ -1112,27 +1210,27 @@
       <c r="G28" s="22"/>
       <c r="H28" s="23"/>
     </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="24"/>
+      <c r="F30" s="25"/>
       <c r="G30" s="6"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="b">
         <v>1</v>
       </c>
@@ -1144,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
       <c r="E32" s="17"/>
@@ -1154,7 +1252,7 @@
       <c r="G32" s="16"/>
       <c r="H32" s="17"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
       <c r="E33" s="20"/>
@@ -1162,7 +1260,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="21"/>
       <c r="D34" s="22"/>
       <c r="E34" s="23"/>
@@ -1170,27 +1268,27 @@
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F36" s="24"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="6"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="8" t="b">
         <v>1</v>
       </c>
@@ -1202,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
       <c r="E38" s="17"/>
@@ -1212,7 +1310,7 @@
       <c r="G38" s="16"/>
       <c r="H38" s="17"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="18"/>
       <c r="D39" s="19"/>
       <c r="E39" s="20"/>
@@ -1220,7 +1318,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="21"/>
       <c r="D40" s="22"/>
       <c r="E40" s="23"/>
@@ -1228,27 +1326,27 @@
       <c r="G40" s="22"/>
       <c r="H40" s="23"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F42" s="24"/>
+      <c r="F42" s="25"/>
       <c r="G42" s="6"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="8" t="b">
         <v>1</v>
       </c>
@@ -1260,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="15"/>
       <c r="D44" s="16"/>
       <c r="E44" s="17"/>
@@ -1270,7 +1368,7 @@
       <c r="G44" s="16"/>
       <c r="H44" s="17"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="18"/>
       <c r="D45" s="19"/>
       <c r="E45" s="20"/>
@@ -1278,7 +1376,7 @@
       <c r="G45" s="19"/>
       <c r="H45" s="20"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="21"/>
       <c r="D46" s="22"/>
       <c r="E46" s="23"/>
@@ -1286,27 +1384,27 @@
       <c r="G46" s="22"/>
       <c r="H46" s="23"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="24"/>
+      <c r="F48" s="25"/>
       <c r="G48" s="6"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="8" t="b">
         <v>1</v>
       </c>
@@ -1318,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="15" t="s">
         <v>13</v>
       </c>
@@ -1328,7 +1426,7 @@
       <c r="G50" s="16"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" s="18"/>
       <c r="D51" s="19"/>
       <c r="E51" s="20"/>
@@ -1336,7 +1434,7 @@
       <c r="G51" s="19"/>
       <c r="H51" s="20"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52" s="21"/>
       <c r="D52" s="22"/>
       <c r="E52" s="23"/>
@@ -1346,18 +1444,10 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C44:E46"/>
-    <mergeCell ref="F44:H46"/>
-    <mergeCell ref="C50:E52"/>
-    <mergeCell ref="F50:H52"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C38:E40"/>
-    <mergeCell ref="F38:H40"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="C32:E34"/>
+    <mergeCell ref="F32:H34"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="D29:G29"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D20:G20"/>
@@ -1373,10 +1463,18 @@
     <mergeCell ref="F14:H16"/>
     <mergeCell ref="F17:H19"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C32:E34"/>
-    <mergeCell ref="F32:H34"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C44:E46"/>
+    <mergeCell ref="F44:H46"/>
+    <mergeCell ref="C50:E52"/>
+    <mergeCell ref="F50:H52"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C38:E40"/>
+    <mergeCell ref="F38:H40"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="D47:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="88" orientation="portrait" r:id="rId1"/>

</xml_diff>